<commit_message>
Datos para el estudio.
</commit_message>
<xml_diff>
--- a/Reservas_Quarzo_Novazul.xlsx
+++ b/Reservas_Quarzo_Novazul.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diacon\Desktop\Estudios\EstudioActuarialFomentoUrbano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5127AF73-7994-4AF1-91A1-F97929FC6EDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C63DEA-A93E-40E6-AED7-F76F922908EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1FBEEA0-F1A4-4B0C-810A-6DC0D38E29FF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="36">
   <si>
     <t>Proy</t>
   </si>
@@ -54,418 +54,91 @@
     <t>feb</t>
   </si>
   <si>
-    <t>CASA #76 CITRINO 2D</t>
-  </si>
-  <si>
-    <t>CASA #78 CITRINO 3D 2.0</t>
-  </si>
-  <si>
-    <t>CASA #85 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #87 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #90 CITRINO 2D</t>
-  </si>
-  <si>
     <t>mar</t>
   </si>
   <si>
-    <t>CASA #65 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #89 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #91 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #92 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #93 AMATISTA 3D</t>
-  </si>
-  <si>
     <t>may</t>
   </si>
   <si>
-    <t>CASA #88 CITRINO 3D</t>
-  </si>
-  <si>
     <t>jun</t>
   </si>
   <si>
-    <t>CASA #77 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #84 CITRINO 3D</t>
-  </si>
-  <si>
     <t>jul</t>
   </si>
   <si>
-    <t>CASA #83 CITRINO 3D</t>
-  </si>
-  <si>
     <t>ago</t>
   </si>
   <si>
-    <t>CASA #1 CITRINO 3 D 128.5 M2</t>
-  </si>
-  <si>
-    <t>CASA #68 CITRINO 2D</t>
-  </si>
-  <si>
-    <t>CASA #75 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #81 CITRINO 2D</t>
-  </si>
-  <si>
     <t>sep</t>
   </si>
   <si>
-    <t>CASA #10 CITRINO 2D</t>
-  </si>
-  <si>
-    <t>CASA #69 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #70 CITRINO 3D</t>
-  </si>
-  <si>
     <t>dic</t>
   </si>
   <si>
-    <t>CASA #16 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #7 OPALO</t>
-  </si>
-  <si>
     <t>2018</t>
   </si>
   <si>
     <t>ene</t>
   </si>
   <si>
-    <t>CASA #73 CITRINO 2D</t>
-  </si>
-  <si>
-    <t>CASA #71 CITRINO 2D 2.0</t>
-  </si>
-  <si>
-    <t>CASA #86 AMATISTA 2D</t>
-  </si>
-  <si>
-    <t>CASA # 12 CITRINO 3D 2.0</t>
-  </si>
-  <si>
-    <t>CASA # 8 OPALO</t>
-  </si>
-  <si>
-    <t>CASA # 9 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #11 CITRINO 3D 2.0</t>
-  </si>
-  <si>
-    <t>CASA #14 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #2 CITRINO 2D</t>
-  </si>
-  <si>
-    <t>CASA #5 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #72 CITRINO 2D</t>
-  </si>
-  <si>
-    <t>CASA #74 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #80 CITRINO 2D 2.0</t>
-  </si>
-  <si>
-    <t>CASA #82 CITRINO 2D</t>
-  </si>
-  <si>
     <t>abr</t>
   </si>
   <si>
-    <t>CASA #13 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #4 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #51 AMATISTA 2D</t>
-  </si>
-  <si>
-    <t>CASA #03 CITRINO 3D 2.0</t>
-  </si>
-  <si>
-    <t>CASA #40 OPALO AJUSTADA</t>
-  </si>
-  <si>
-    <t>CASA #06 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #15 OPALO</t>
-  </si>
-  <si>
-    <t>CSASA #18 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #55 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #59 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #60 CITRINO 3D 2.0</t>
-  </si>
-  <si>
-    <t>CASA #62 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #17 OPALO</t>
-  </si>
-  <si>
-    <t>CASA #43 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #44 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #61 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #49 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #56 CITRINO 3D</t>
-  </si>
-  <si>
     <t>oct</t>
   </si>
   <si>
-    <t>CASA #41 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #48 AMATISTA 2D</t>
-  </si>
-  <si>
-    <t>CASA 53 CITRINO 3 d</t>
-  </si>
-  <si>
     <t>2019</t>
   </si>
   <si>
-    <t>CASA 57 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA 58 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #45 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #63 CITRINO</t>
-  </si>
-  <si>
-    <t>CASA #23 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #63 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #47 AMATISTA 3D</t>
-  </si>
-  <si>
-    <t>CASA #25 CITRINO 3DOR</t>
-  </si>
-  <si>
     <t>nov</t>
   </si>
   <si>
-    <t>CASA #35 CITRINO 3DOR</t>
-  </si>
-  <si>
-    <t>CASA #28 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #54 CITRINO 3D</t>
-  </si>
-  <si>
     <t>2020</t>
   </si>
   <si>
-    <t>CASA #79 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #50 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #36 AMATISTA 2D</t>
-  </si>
-  <si>
-    <t>CASA #22 CITRNO 3D</t>
-  </si>
-  <si>
-    <t>CASA #27 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #29 AMATISTA 3 D</t>
-  </si>
-  <si>
-    <t>CASA # 39 AMATISTA 151.63 M2 3 DORM.</t>
-  </si>
-  <si>
     <t>Novazul</t>
   </si>
   <si>
-    <t xml:space="preserve">CASA #23 CITRINO 3D </t>
-  </si>
-  <si>
-    <t>FM 05 CASA 84 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>FM 05 CASA 12 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA 87 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA 98 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA 90 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA 93 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA 96 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA #94 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA #12 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 02 CASA #113 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 15 CASA 08 ALTADENA</t>
-  </si>
-  <si>
-    <t>FM 02 CASA 114 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 02 CASA 116 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA 91 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA 104 FM3 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 02 CASA 115 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>FM 02 CASA 117 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>FM 04 CASA 92 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM3 CASA 105 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM3 CASA 106 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM 11 LOTE 13 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>LOTE 04 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM15 CASA #6 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>FM15 CASA #04 ALTADENA 3D</t>
-  </si>
-  <si>
-    <t>FM2  CASA #120 ALTADENA 3D</t>
-  </si>
-  <si>
-    <t>FM3 CASA ·107 CITRINO 3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FM3 CASA #103 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #07 ALTADENA 3D</t>
-  </si>
-  <si>
-    <t>FM3 CASA #111 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #109 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>CASA #97 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>CASA #118 3D NOVAZUL</t>
-  </si>
-  <si>
-    <t>CASA 101 CITRINO</t>
-  </si>
-  <si>
-    <t>LOTE #15 CITRINO 3D</t>
-  </si>
-  <si>
-    <t>CASA #64 NOVAZUL</t>
-  </si>
-  <si>
-    <t>CASA #112 CITRINO 3 D</t>
-  </si>
-  <si>
-    <t>CASA #63 CITRINO 3DOR</t>
-  </si>
-  <si>
-    <t>CASA 89 NOVAZUL 2D</t>
-  </si>
-  <si>
-    <t>FM 03 CASA 102 AMBAR 2D</t>
-  </si>
-  <si>
-    <t>LOTE 22 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>CASA 110 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>LOTE 24 NOVAZUL 2D</t>
-  </si>
-  <si>
-    <t>CASA #67 NOVAZUL 3D</t>
-  </si>
-  <si>
-    <t>CASA #77 TIPO CITRINO A-190657-F000</t>
-  </si>
-  <si>
-    <t>CASA #82 TIPO NOVAZUL 2-192074-F-000</t>
-  </si>
-  <si>
-    <t>CASA #69 CITRINO 3DOR</t>
+    <t>CITRINO 2D</t>
+  </si>
+  <si>
+    <t>CITRINO 3D 2.0</t>
+  </si>
+  <si>
+    <t>AMATISTA 3D</t>
+  </si>
+  <si>
+    <t>OPALO</t>
+  </si>
+  <si>
+    <t>CITRINO 3D</t>
+  </si>
+  <si>
+    <t>CITRINO 2D 2.0</t>
+  </si>
+  <si>
+    <t>AMATISTA 2D</t>
+  </si>
+  <si>
+    <t>CITRINO</t>
+  </si>
+  <si>
+    <t>NOVAZUL 3D</t>
+  </si>
+  <si>
+    <t>NOVAZUL 2D</t>
+  </si>
+  <si>
+    <t>AMBAR 2D</t>
+  </si>
+  <si>
+    <t>NOVAZUL</t>
+  </si>
+  <si>
+    <t>ALTADENA 3D</t>
+  </si>
+  <si>
+    <t>ALTADENA</t>
   </si>
 </sst>
 </file>
@@ -848,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45937C5E-2535-4B78-A430-6783994802F3}">
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +552,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,7 +566,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,7 +580,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,7 +594,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -935,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -946,10 +619,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -960,10 +633,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -974,10 +647,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -988,10 +661,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1002,10 +675,10 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,10 +689,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1030,10 +703,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1044,10 +717,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1058,10 +731,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1072,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
@@ -1086,10 +759,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1100,10 +773,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1114,10 +787,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,10 +801,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,10 +815,10 @@
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1156,10 +829,10 @@
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1170,10 +843,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1184,10 +857,10 @@
         <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1195,13 +868,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1209,13 +882,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1223,13 +896,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1237,13 +910,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1251,13 +924,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1265,13 +938,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1279,13 +952,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1293,13 +966,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1307,13 +980,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1321,13 +994,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1335,13 +1008,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1349,13 +1022,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,13 +1036,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1377,13 +1050,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1391,13 +1064,13 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1405,13 +1078,13 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1419,13 +1092,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1433,13 +1106,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1447,13 +1120,13 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1461,13 +1134,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1475,13 +1148,13 @@
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1489,13 +1162,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1503,13 +1176,13 @@
         <v>4</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1517,13 +1190,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1531,13 +1204,13 @@
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1545,13 +1218,13 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1559,13 +1232,13 @@
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1573,13 +1246,13 @@
         <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1587,13 +1260,13 @@
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1601,13 +1274,13 @@
         <v>4</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1615,13 +1288,13 @@
         <v>4</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1629,13 +1302,13 @@
         <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1643,13 +1316,13 @@
         <v>4</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1657,13 +1330,13 @@
         <v>4</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,13 +1344,13 @@
         <v>4</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1685,13 +1358,13 @@
         <v>4</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1699,13 +1372,13 @@
         <v>4</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1713,13 +1386,13 @@
         <v>4</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1727,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1741,13 +1414,13 @@
         <v>4</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1755,13 +1428,13 @@
         <v>4</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1769,13 +1442,13 @@
         <v>4</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1783,13 +1456,13 @@
         <v>4</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1797,13 +1470,13 @@
         <v>4</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1811,13 +1484,13 @@
         <v>4</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1825,13 +1498,13 @@
         <v>4</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1839,13 +1512,13 @@
         <v>4</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1853,13 +1526,13 @@
         <v>4</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1867,13 +1540,13 @@
         <v>4</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1881,13 +1554,13 @@
         <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1895,13 +1568,13 @@
         <v>4</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,13 +1582,13 @@
         <v>4</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1923,13 +1596,13 @@
         <v>4</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1937,685 +1610,685 @@
         <v>4</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>102</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>114</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>116</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>118</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>120</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>121</v>
+        <v>26</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>122</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>127</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>129</v>
+        <v>30</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>131</v>
+        <v>29</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>132</v>
+        <v>26</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>138</v>
+        <v>30</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>144</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>